<commit_message>
Business Plan for Financial Summary Report
</commit_message>
<xml_diff>
--- a/Documents/Finance/Financial Summary Report/Business plan.xlsx
+++ b/Documents/Finance/Financial Summary Report/Business plan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="17560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Buisness Projection" sheetId="1" r:id="rId1"/>
@@ -606,7 +606,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -795,6 +795,10 @@
     <xf numFmtId="4" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="3" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -810,7 +814,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="38">
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
@@ -1182,57 +1193,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:209" ht="59.25" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
-      <c r="V1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
     </row>
     <row r="2" spans="1:209" ht="18">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
       <c r="G2" s="9"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="112" t="s">
+      <c r="J2" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="116" t="s">
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="114"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
+      <c r="Q2" s="114"/>
+      <c r="R2" s="114"/>
+      <c r="S2" s="114"/>
+      <c r="T2" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="116"/>
+      <c r="U2" s="118"/>
       <c r="V2" s="66"/>
       <c r="W2" s="66"/>
       <c r="X2" s="66"/>
@@ -4348,11 +4359,11 @@
     </row>
     <row r="38" spans="1:109">
       <c r="A38" s="3"/>
-      <c r="J38" s="113" t="s">
+      <c r="J38" s="115" t="s">
         <v>38</v>
       </c>
-      <c r="K38" s="113"/>
-      <c r="L38" s="114"/>
+      <c r="K38" s="115"/>
+      <c r="L38" s="116"/>
       <c r="M38" s="92"/>
       <c r="N38" s="94"/>
       <c r="O38" s="17" t="s">
@@ -4515,7 +4526,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="B22" sqref="B22:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5337,20 +5348,20 @@
       <c r="A22" s="73">
         <v>41764</v>
       </c>
-      <c r="B22" s="78">
+      <c r="B22" s="119">
         <v>3</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="104"/>
-      <c r="G22" s="77"/>
-      <c r="H22" s="104"/>
-      <c r="I22" s="77"/>
-      <c r="J22" s="77"/>
-      <c r="K22" s="104"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="13">
+      <c r="C22" s="120"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="120"/>
+      <c r="G22" s="120"/>
+      <c r="H22" s="120"/>
+      <c r="I22" s="120"/>
+      <c r="J22" s="120"/>
+      <c r="K22" s="120"/>
+      <c r="L22" s="120"/>
+      <c r="M22" s="121">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5359,20 +5370,20 @@
       <c r="A23" s="73">
         <v>41771</v>
       </c>
-      <c r="B23" s="76">
+      <c r="B23" s="122">
         <v>4</v>
       </c>
-      <c r="C23" s="104"/>
-      <c r="D23" s="104"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="104"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="104"/>
-      <c r="I23" s="104"/>
-      <c r="J23" s="104"/>
-      <c r="K23" s="104"/>
-      <c r="L23" s="104"/>
-      <c r="M23" s="13">
+      <c r="C23" s="120"/>
+      <c r="D23" s="120"/>
+      <c r="E23" s="120"/>
+      <c r="F23" s="120"/>
+      <c r="G23" s="120"/>
+      <c r="H23" s="120"/>
+      <c r="I23" s="120"/>
+      <c r="J23" s="120"/>
+      <c r="K23" s="120"/>
+      <c r="L23" s="120"/>
+      <c r="M23" s="121">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5381,20 +5392,20 @@
       <c r="A24" s="73">
         <v>41778</v>
       </c>
-      <c r="B24" s="83">
+      <c r="B24" s="112">
         <v>5</v>
       </c>
-      <c r="C24" s="104"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="104"/>
-      <c r="G24" s="104"/>
-      <c r="H24" s="104"/>
-      <c r="I24" s="104"/>
-      <c r="J24" s="104"/>
-      <c r="K24" s="104"/>
-      <c r="L24" s="104"/>
-      <c r="M24" s="13">
+      <c r="C24" s="120"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="120"/>
+      <c r="G24" s="120"/>
+      <c r="H24" s="120"/>
+      <c r="I24" s="120"/>
+      <c r="J24" s="120"/>
+      <c r="K24" s="120"/>
+      <c r="L24" s="120"/>
+      <c r="M24" s="121">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5573,7 +5584,7 @@
       </c>
     </row>
     <row r="38" spans="3:13">
-      <c r="C38" s="117">
+      <c r="C38" s="113">
         <f>((C37/12.5)/10)/5</f>
         <v>7.6796000000000006</v>
       </c>

</xml_diff>